<commit_message>
mejoras en el modulo de entrada analógico
</commit_message>
<xml_diff>
--- a/entrada analógica/memoryMaps.xlsx
+++ b/entrada analógica/memoryMaps.xlsx
@@ -173,34 +173,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -509,7 +509,7 @@
   <dimension ref="A1:L101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,104 +520,104 @@
     <col min="4" max="4" width="103.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="7">
         <v>0</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="7">
         <v>1</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="7">
         <v>2</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="7">
         <v>3</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="7">
         <v>0</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="7">
         <v>0</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="11" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="7">
         <v>0</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="7">
         <v>3648</v>
       </c>
       <c r="D9" s="13" t="s">
@@ -625,35 +625,35 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="7">
         <v>3649</v>
       </c>
       <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="7">
         <v>3650</v>
       </c>
       <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="7">
         <v>3651</v>
       </c>
       <c r="D12" s="13"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="7">
         <v>3652</v>
       </c>
       <c r="D13" s="13" t="s">
@@ -661,35 +661,35 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="7">
         <v>3653</v>
       </c>
       <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="7">
         <v>3654</v>
       </c>
       <c r="D15" s="13"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="7">
         <v>3655</v>
       </c>
       <c r="D16" s="13"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="7">
         <v>3656</v>
       </c>
       <c r="D17" s="13" t="s">
@@ -697,35 +697,35 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="14"/>
-      <c r="C18" s="9">
+      <c r="C18" s="7">
         <v>3657</v>
       </c>
       <c r="D18" s="13"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="14"/>
-      <c r="C19" s="9">
+      <c r="C19" s="7">
         <v>3658</v>
       </c>
       <c r="D19" s="13"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="14"/>
-      <c r="C20" s="9">
+      <c r="C20" s="7">
         <v>3659</v>
       </c>
       <c r="D20" s="13"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8" t="s">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="7">
         <v>3660</v>
       </c>
       <c r="D21" s="13" t="s">
@@ -733,25 +733,25 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="7">
         <v>3661</v>
       </c>
       <c r="D22" s="13"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="9">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="7">
         <v>3662</v>
       </c>
       <c r="D23" s="13"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="7">
         <v>3663</v>
       </c>
       <c r="D24" s="13"/>
@@ -823,42 +823,42 @@
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="7"/>
+      <c r="D41" s="6"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="7"/>
+      <c r="D42" s="6"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="7"/>
+      <c r="D43" s="6"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="7"/>
+      <c r="D44" s="6"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="7"/>
+      <c r="D45" s="6"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="7"/>
+      <c r="D46" s="6"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="7"/>
+      <c r="D47" s="6"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="7"/>
+      <c r="D48" s="6"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
@@ -985,7 +985,7 @@
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C94" s="1">
@@ -993,25 +993,25 @@
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="5"/>
+      <c r="B95" s="12"/>
       <c r="C95" s="1">
         <v>3673</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B96" s="5"/>
+      <c r="B96" s="12"/>
       <c r="C96" s="1">
         <v>3674</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B97" s="5"/>
+      <c r="B97" s="12"/>
       <c r="C97" s="1">
         <v>3675</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="5" t="s">
+      <c r="B98" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C98" s="1">
@@ -1019,40 +1019,40 @@
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B99" s="5"/>
+      <c r="B99" s="12"/>
       <c r="C99" s="1">
         <v>3677</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="5"/>
+      <c r="B100" s="12"/>
       <c r="C100" s="1">
         <v>3678</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B101" s="5"/>
+      <c r="B101" s="12"/>
       <c r="C101" s="1">
         <v>3679</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D21:D24"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="D9:D12"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A24"/>
     <mergeCell ref="B98:B101"/>
     <mergeCell ref="B21:B24"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="D9:D12"/>
     <mergeCell ref="B94:B97"/>
-    <mergeCell ref="D21:D24"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="D2:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>